<commit_message>
Changes to names and docstrings
</commit_message>
<xml_diff>
--- a/src/data/paralympics.xlsx
+++ b/src/data/paralympics.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10102"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10208"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sarahsanders/PycharmProjects/comp0034-tutorialapp-dash/src/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sarahsanders/PycharmProjects/comp0034_tutorialapp_fastapi/src/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CDF196E-999A-0849-9E23-A560B6274290}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E210A27E-7395-EF45-970C-F28E08EF0A17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2200" yWindow="680" windowWidth="28040" windowHeight="17200" xr2:uid="{CBF15B4E-2805-CD44-9DA6-567684115F1A}"/>
   </bookViews>
@@ -3461,7 +3461,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="5" topLeftCell="Q1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="Q9" sqref="Q9:R9"/>
+      <selection pane="topRight" activeCell="U20" sqref="U20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5446,7 +5446,7 @@
   <dimension ref="A1:F233"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+      <selection activeCell="I253" sqref="I253"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>